<commit_message>
Use "short" error codes for config files
</commit_message>
<xml_diff>
--- a/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
+++ b/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\src\PhpSpreadsheet\Calculation\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC82EE7-E78E-43E5-86E0-F7C6B93F2BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B96276-825E-4349-AF5A-109120426D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4406" yWindow="1243" windowWidth="24685" windowHeight="16723" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8604" uniqueCount="6511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8611" uniqueCount="6515">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -19602,6 +19602,18 @@
   </si>
   <si>
     <t>Slovenščina</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>REF</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>DIV0</t>
   </si>
 </sst>
 </file>
@@ -20026,10 +20038,10 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20361,9 +20373,11 @@
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3" t="s">
+        <v>6344</v>
+      </c>
       <c r="B8" s="3" t="s">
-        <v>6344</v>
+        <v>6511</v>
       </c>
       <c r="C8" t="s">
         <v>6352</v>
@@ -20424,8 +20438,11 @@
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A9" s="3" t="s">
+        <v>6471</v>
+      </c>
       <c r="B9" s="3" t="s">
-        <v>6471</v>
+        <v>6514</v>
       </c>
       <c r="C9" t="s">
         <v>6366</v>
@@ -20471,8 +20488,11 @@
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>6472</v>
+      </c>
       <c r="B10" s="3" t="s">
-        <v>6472</v>
+        <v>748</v>
       </c>
       <c r="C10" t="s">
         <v>6380</v>
@@ -20551,8 +20571,11 @@
       </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>6473</v>
+      </c>
       <c r="B11" s="3" t="s">
-        <v>6473</v>
+        <v>6512</v>
       </c>
       <c r="C11" t="s">
         <v>6403</v>
@@ -20604,8 +20627,11 @@
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>6474</v>
+      </c>
       <c r="B12" s="3" t="s">
-        <v>6474</v>
+        <v>6513</v>
       </c>
       <c r="C12" t="s">
         <v>6418</v>
@@ -20681,8 +20707,11 @@
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A13" s="3" t="s">
+        <v>6475</v>
+      </c>
       <c r="B13" s="3" t="s">
-        <v>6475</v>
+        <v>3070</v>
       </c>
       <c r="C13" t="s">
         <v>6437</v>
@@ -20743,8 +20772,11 @@
       </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.4">
+      <c r="A14" s="3" t="s">
+        <v>6476</v>
+      </c>
       <c r="B14" s="3" t="s">
-        <v>6476</v>
+        <v>300</v>
       </c>
       <c r="C14" t="s">
         <v>6453</v>

</xml_diff>

<commit_message>
Additional russian function translations (#2554)
* Additional Russian translations for Excel functions

* Update change log
</commit_message>
<xml_diff>
--- a/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
+++ b/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\src\PhpSpreadsheet\Calculation\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F14B4C-B7A9-4CCB-93EC-FA8A16A75332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48C1BC0-1CE1-483D-8D6D-B0314F47B0D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4406" yWindow="1243" windowWidth="24685" windowHeight="16723" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7123" yWindow="2057" windowWidth="24686" windowHeight="16149" tabRatio="989" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Excel Localisation" sheetId="4" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8611" uniqueCount="6515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8630" uniqueCount="6535">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -19614,13 +19614,73 @@
   </si>
   <si>
     <t>DIV0</t>
+  </si>
+  <si>
+    <t>ДОЛЛСША</t>
+  </si>
+  <si>
+    <t>ФИЛЬТР</t>
+  </si>
+  <si>
+    <t>СОРТ</t>
+  </si>
+  <si>
+    <t>СОРТПО</t>
+  </si>
+  <si>
+    <t>УНИК</t>
+  </si>
+  <si>
+    <t>ПРОСМОТРX</t>
+  </si>
+  <si>
+    <t>ПОИСКПОЗX</t>
+  </si>
+  <si>
+    <t>СЛУЧМАССИВ</t>
+  </si>
+  <si>
+    <t>ПОСЛЕДОВ</t>
+  </si>
+  <si>
+    <t>МАССИВВТЕКСТ</t>
+  </si>
+  <si>
+    <t>БДЦС</t>
+  </si>
+  <si>
+    <t>НАЙТИБ</t>
+  </si>
+  <si>
+    <t>ЛЕВБ</t>
+  </si>
+  <si>
+    <t>ДЛИНБ</t>
+  </si>
+  <si>
+    <t>ПСТРБ</t>
+  </si>
+  <si>
+    <t>ЗАМЕНИТЬБ</t>
+  </si>
+  <si>
+    <t>ПРАВБ</t>
+  </si>
+  <si>
+    <t>ПОИСКБ</t>
+  </si>
+  <si>
+    <t>ЗНАЧЕНИЕВТЕКСТ</t>
+  </si>
+  <si>
+    <t>ЕТАЙЦИФРЫ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -19632,12 +19692,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -19675,10 +19729,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20037,11 +20091,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1A36666-6E7A-4A48-9C4E-B256160FF964}">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20852,11 +20906,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31683534-79D8-42E0-A1E0-6E4CC43822BE}">
   <dimension ref="A1:R526"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="F435" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:A3"/>
+      <selection pane="bottomRight" activeCell="G444" sqref="G444"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -20881,7 +20935,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -20937,7 +20991,7 @@
       </c>
     </row>
     <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="C2" s="2" t="s">
         <v>5768</v>
       </c>
@@ -20988,7 +21042,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>2004</v>
       </c>
@@ -29304,6 +29358,9 @@
       <c r="B164" s="1" t="s">
         <v>6145</v>
       </c>
+      <c r="G164" s="1" t="s">
+        <v>6515</v>
+      </c>
     </row>
     <row r="165" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B165" s="1" t="s">
@@ -31713,6 +31770,9 @@
       <c r="B213" s="1" t="s">
         <v>6081</v>
       </c>
+      <c r="G213" s="1" t="s">
+        <v>6516</v>
+      </c>
     </row>
     <row r="214" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B214" s="1" t="s">
@@ -32355,12 +32415,18 @@
       <c r="B226" s="1" t="s">
         <v>6082</v>
       </c>
+      <c r="G226" s="1" t="s">
+        <v>6517</v>
+      </c>
     </row>
     <row r="227" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A227" s="2"/>
       <c r="B227" s="1" t="s">
         <v>6083</v>
       </c>
+      <c r="G227" s="1" t="s">
+        <v>6518</v>
+      </c>
     </row>
     <row r="228" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B228" s="1" t="s">
@@ -32420,6 +32486,9 @@
       <c r="B229" s="1" t="s">
         <v>6084</v>
       </c>
+      <c r="G229" s="1" t="s">
+        <v>6519</v>
+      </c>
     </row>
     <row r="230" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B230" s="1" t="s">
@@ -32479,12 +32548,18 @@
       <c r="B231" s="1" t="s">
         <v>6085</v>
       </c>
+      <c r="G231" s="1" t="s">
+        <v>6520</v>
+      </c>
     </row>
     <row r="232" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A232" s="2"/>
       <c r="B232" s="1" t="s">
         <v>6086</v>
       </c>
+      <c r="G232" s="1" t="s">
+        <v>6521</v>
+      </c>
     </row>
     <row r="233" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A233" s="2"/>
@@ -35351,6 +35426,9 @@
       <c r="B288" s="1" t="s">
         <v>6090</v>
       </c>
+      <c r="G288" s="1" t="s">
+        <v>6522</v>
+      </c>
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B289" s="1" t="s">
@@ -35871,6 +35949,9 @@
       <c r="B299" s="1" t="s">
         <v>6091</v>
       </c>
+      <c r="G299" s="1" t="s">
+        <v>6523</v>
+      </c>
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B300" s="1" t="s">
@@ -42721,17 +42802,20 @@
         <v>5911</v>
       </c>
     </row>
-    <row r="431" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B431" s="5" t="s">
+    <row r="431" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B431" s="4" t="s">
         <v>6092</v>
       </c>
-      <c r="R431" s="5" t="s">
+      <c r="R431" s="4" t="s">
         <v>6113</v>
       </c>
     </row>
-    <row r="432" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B432" s="5" t="s">
+    <row r="432" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B432" s="4" t="s">
         <v>6093</v>
+      </c>
+      <c r="G432" s="4" t="s">
+        <v>6524</v>
       </c>
     </row>
     <row r="433" spans="1:18" x14ac:dyDescent="0.4">
@@ -43004,6 +43088,9 @@
       <c r="B438" s="1" t="s">
         <v>6094</v>
       </c>
+      <c r="G438" s="1" t="s">
+        <v>6525</v>
+      </c>
     </row>
     <row r="439" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B439" s="1" t="s">
@@ -43169,6 +43256,9 @@
       <c r="B442" s="1" t="s">
         <v>6095</v>
       </c>
+      <c r="G442" s="1" t="s">
+        <v>6526</v>
+      </c>
     </row>
     <row r="443" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B443" s="1" t="s">
@@ -43235,7 +43325,7 @@
         <v>6190</v>
       </c>
       <c r="G444" s="1" t="s">
-        <v>6190</v>
+        <v>6534</v>
       </c>
       <c r="H444" s="1" t="s">
         <v>6191</v>
@@ -43323,6 +43413,9 @@
       <c r="B446" s="1" t="s">
         <v>6096</v>
       </c>
+      <c r="G446" s="1" t="s">
+        <v>6527</v>
+      </c>
     </row>
     <row r="447" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B447" s="1" t="s">
@@ -43382,6 +43475,9 @@
       <c r="B448" s="1" t="s">
         <v>6097</v>
       </c>
+      <c r="G448" s="1" t="s">
+        <v>6528</v>
+      </c>
     </row>
     <row r="449" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B449" s="1" t="s">
@@ -43494,6 +43590,9 @@
       <c r="B451" s="1" t="s">
         <v>6098</v>
       </c>
+      <c r="G451" s="1" t="s">
+        <v>6529</v>
+      </c>
     </row>
     <row r="452" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A452" s="2"/>
@@ -43743,6 +43842,9 @@
       <c r="B457" s="1" t="s">
         <v>6100</v>
       </c>
+      <c r="G457" s="1" t="s">
+        <v>6530</v>
+      </c>
     </row>
     <row r="458" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B458" s="1" t="s">
@@ -43855,6 +43957,9 @@
       <c r="B460" s="1" t="s">
         <v>6101</v>
       </c>
+      <c r="G460" s="1" t="s">
+        <v>6531</v>
+      </c>
     </row>
     <row r="461" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B461" s="1" t="s">
@@ -43914,6 +44019,9 @@
       <c r="B462" s="1" t="s">
         <v>6102</v>
       </c>
+      <c r="G462" s="1" t="s">
+        <v>6532</v>
+      </c>
     </row>
     <row r="463" spans="1:18" x14ac:dyDescent="0.4">
       <c r="B463" s="1" t="s">
@@ -44576,6 +44684,9 @@
       <c r="A476" s="2"/>
       <c r="B476" s="1" t="s">
         <v>6103</v>
+      </c>
+      <c r="G476" s="1" t="s">
+        <v>6533</v>
       </c>
     </row>
     <row r="477" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Some Bulgarian Function Omissions
Figured out a reasonable way to compare old Bulgarian function file to new; this identified a handful of now-corrected omissions and errors. Note that JIS function, in old list, is not on spreadsheet, but the Bulgarian translation is the same as English (so the translation isn't needed), and the function has been replaced by DBCS, which is also not on the spreadsheet.
</commit_message>
<xml_diff>
--- a/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
+++ b/src/PhpSpreadsheet/Calculation/locale/Translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nooctal3\src\PhpSpreadsheet\Calculation\locale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\nooctal\src\PhpSpreadsheet\Calculation\locale\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F63CE09-D370-4A1D-AF32-D497C4E7ECD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E7E357-BC02-47A7-9FD9-A058D7403D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="989" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,6 +63,7 @@
     <author>tc={FF6A9B1E-172D-419A-AE26-363E0061308C}</author>
     <author>tc={CACDDDBD-012F-4F2F-8457-4FF52EB4D2D0}</author>
     <author>tc={3B6725E7-9A95-45C6-BAD0-BB4C900C4B9F}</author>
+    <author>tc={6005DC7F-03C9-4B1E-B445-787F12B5B7BC}</author>
     <author>tc={5539F2F5-C7CE-40CC-84E7-73C614DD1C3A}</author>
     <author>tc={0BC0B73F-15BC-4022-959C-D8A0FF6F60FB}</author>
     <author>tc={4BB940B1-F984-4562-9953-F98AB6C81E95}</author>
@@ -312,7 +313,17 @@
 VLOOKUP			= ВПР					##	Ищет значение в первом столбце массива и возвращает значение из ячейки в найденной строке и указанном столбце.</t>
       </text>
     </comment>
-    <comment ref="S244" authorId="10" shapeId="0" xr:uid="{5539F2F5-C7CE-40CC-84E7-73C614DD1C3A}">
+    <comment ref="S224" authorId="10" shapeId="0" xr:uid="{6005DC7F-03C9-4B1E-B445-787F12B5B7BC}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    ##	Add-in and Automation functions				Функции надстроек и автоматизации
+##
+GETPIVOTDATA		= ПОЛУЧИТЬ.ДАННЫЕ.СВОДНОЙ.ТАБЛИЦЫ	##	Возвращает данные, хранящиеся в отчете сводной таблицы.</t>
+      </text>
+    </comment>
+    <comment ref="S244" authorId="11" shapeId="0" xr:uid="{5539F2F5-C7CE-40CC-84E7-73C614DD1C3A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -379,7 +390,7 @@
 TRUNC			= ОТБР					##	Отбрасывает дробную часть числа.</t>
       </text>
     </comment>
-    <comment ref="S339" authorId="11" shapeId="0" xr:uid="{0BC0B73F-15BC-4022-959C-D8A0FF6F60FB}">
+    <comment ref="S339" authorId="12" shapeId="0" xr:uid="{0BC0B73F-15BC-4022-959C-D8A0FF6F60FB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -469,7 +480,7 @@
 ZTEST			= ZТЕСТ					##	Возвращает двустороннее P-значение z-теста.</t>
       </text>
     </comment>
-    <comment ref="S451" authorId="12" shapeId="0" xr:uid="{4BB940B1-F984-4562-9953-F98AB6C81E95}">
+    <comment ref="S451" authorId="13" shapeId="0" xr:uid="{4BB940B1-F984-4562-9953-F98AB6C81E95}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -515,7 +526,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9042" uniqueCount="6579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9046" uniqueCount="6579">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -20855,6 +20866,11 @@
 TRANSPOSE		= ТРАНСП				##	Возвращает транспонированный массив.
 VLOOKUP			= ВПР					##	Ищет значение в первом столбце массива и возвращает значение из ячейки в найденной строке и указанном столбце.</text>
   </threadedComment>
+  <threadedComment ref="S224" dT="2023-08-22T20:04:15.97" personId="{EAE7CA6B-11B8-4DE7-B323-DC98103C3602}" id="{6005DC7F-03C9-4B1E-B445-787F12B5B7BC}">
+    <text>##	Add-in and Automation functions				Функции надстроек и автоматизации
+##
+GETPIVOTDATA		= ПОЛУЧИТЬ.ДАННЫЕ.СВОДНОЙ.ТАБЛИЦЫ	##	Возвращает данные, хранящиеся в отчете сводной таблицы.</text>
+  </threadedComment>
   <threadedComment ref="S244" dT="2023-08-22T02:57:41.82" personId="{EAE7CA6B-11B8-4DE7-B323-DC98103C3602}" id="{5539F2F5-C7CE-40CC-84E7-73C614DD1C3A}">
     <text>ABS			= ABS					##	Возвращает модуль (абсолютную величину) числа.
 ACOS			= ACOS					##	Возвращает арккосинус числа.
@@ -21067,7 +21083,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2510" ySplit="1160" topLeftCell="R4" activePane="topRight"/>
-      <selection pane="topRight" activeCell="AC1" sqref="AC1:AC3"/>
+      <selection pane="topRight" activeCell="AC3" sqref="AC3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
     </sheetView>
@@ -21942,10 +21958,10 @@
   <dimension ref="A1:S550"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5260" ySplit="1160" topLeftCell="R494" activePane="topRight"/>
+      <pane xSplit="5260" ySplit="1160" topLeftCell="Q4" activePane="bottomRight"/>
       <selection pane="topRight" activeCell="S1" sqref="S1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="S451" sqref="S451"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35894,6 +35910,9 @@
       <c r="R278" t="s">
         <v>3805</v>
       </c>
+      <c r="S278" t="s">
+        <v>4538</v>
+      </c>
     </row>
     <row r="279" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B279" t="s">
@@ -44552,6 +44571,9 @@
       </c>
       <c r="R446" t="s">
         <v>3901</v>
+      </c>
+      <c r="S446" t="s">
+        <v>4681</v>
       </c>
     </row>
     <row r="447" spans="2:19" x14ac:dyDescent="0.35">
@@ -47250,6 +47272,9 @@
       <c r="R512" t="s">
         <v>3927</v>
       </c>
+      <c r="S512" t="s">
+        <v>4718</v>
+      </c>
     </row>
     <row r="513" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B513" t="s">
@@ -47863,6 +47888,9 @@
       <c r="R523" t="s">
         <v>3935</v>
       </c>
+      <c r="S523" t="s">
+        <v>4729</v>
+      </c>
     </row>
     <row r="524" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B524" t="s">
@@ -48981,7 +49009,7 @@
         <v>3943</v>
       </c>
       <c r="S543" t="s">
-        <v>4669</v>
+        <v>4749</v>
       </c>
     </row>
     <row r="544" spans="2:19" x14ac:dyDescent="0.35">

</xml_diff>